<commit_message>
La til gitignore fil
</commit_message>
<xml_diff>
--- a/timeliste.xlsx
+++ b/timeliste.xlsx
@@ -10,7 +10,7 @@
   <sheets>
     <sheet name="Sheet2" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="19">
   <si>
     <t xml:space="preserve">Person</t>
   </si>
@@ -59,6 +59,24 @@
   </si>
   <si>
     <t xml:space="preserve">Arbeid med underveisrapport</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Christian</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kode html og css</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Iselin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Går nøye igennom prosjektoppgaven</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kladd nettstedskart, forslag til navn Cruise</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kode html</t>
   </si>
 </sst>
 </file>
@@ -488,32 +506,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I27"/>
+  <dimension ref="A2:I27"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F7" activeCellId="0" sqref="F7"/>
+      <selection pane="topLeft" activeCell="F14" activeCellId="0" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="36.68"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="17.64"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="20.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="3" width="18.61"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="27.78"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="36.71"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="11.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="17.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="20.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="3" width="18.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="27.71"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C1" s="0"/>
-      <c r="D1" s="0"/>
-      <c r="E1" s="0"/>
-      <c r="F1" s="0"/>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -537,10 +546,10 @@
       </c>
       <c r="I2" s="5" t="n">
         <f aca="false">SUM(F3:F27)</f>
-        <v>0.173611111111111</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.881944444444443</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="s">
         <v>7</v>
       </c>
@@ -558,10 +567,10 @@
       </c>
       <c r="F3" s="5" t="n">
         <f aca="false">E3-D3</f>
-        <v>0.0208333333333334</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.020833333333333</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="s">
         <v>9</v>
       </c>
@@ -579,10 +588,10 @@
       </c>
       <c r="F4" s="5" t="n">
         <f aca="false">E4-D4</f>
-        <v>0.0416666666666666</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.041666666666667</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="6" t="s">
         <v>7</v>
       </c>
@@ -600,10 +609,10 @@
       </c>
       <c r="F5" s="5" t="n">
         <f aca="false">E5-D5</f>
-        <v>0.0694444444444444</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.0694444444444442</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="6" t="s">
         <v>7</v>
       </c>
@@ -621,10 +630,10 @@
       </c>
       <c r="F6" s="5" t="n">
         <f aca="false">E6-D6</f>
-        <v>0.0208333333333334</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.020833333333333</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="9" t="s">
         <v>7</v>
       </c>
@@ -642,87 +651,157 @@
       </c>
       <c r="F7" s="5" t="n">
         <f aca="false">E7-D7</f>
-        <v>0.0208333333333334</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="6"/>
-      <c r="B8" s="6"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
+        <v>0.020833333333333</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="7" t="n">
+        <v>43742</v>
+      </c>
+      <c r="D8" s="8" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="E8" s="8" t="n">
+        <v>0.666666666666667</v>
+      </c>
       <c r="F8" s="5" t="n">
         <f aca="false">E8-D8</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="6"/>
-      <c r="B9" s="6"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
+        <v>0.291666666666667</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="7" t="n">
+        <v>43559</v>
+      </c>
+      <c r="D9" s="8" t="n">
+        <v>0.854166666666667</v>
+      </c>
+      <c r="E9" s="8" t="n">
+        <v>0.895833333333333</v>
+      </c>
       <c r="F9" s="5" t="n">
         <f aca="false">E9-D9</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="6"/>
-      <c r="B10" s="6"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
+        <v>0.0416666666666667</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="7" t="n">
+        <v>43562</v>
+      </c>
+      <c r="D10" s="8" t="n">
+        <v>0.875</v>
+      </c>
+      <c r="E10" s="8" t="n">
+        <v>0.958333333333333</v>
+      </c>
       <c r="F10" s="5" t="n">
         <f aca="false">E10-D10</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="6"/>
-      <c r="B11" s="6"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
+        <v>0.0833333333333331</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="7" t="n">
+        <v>43564</v>
+      </c>
+      <c r="D11" s="8" t="n">
+        <v>0.854166666666667</v>
+      </c>
+      <c r="E11" s="8" t="n">
+        <v>1</v>
+      </c>
       <c r="F11" s="5" t="n">
         <f aca="false">E11-D11</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="6"/>
-      <c r="B12" s="6"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
+        <v>0.145833333333333</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="7" t="n">
+        <v>43565</v>
+      </c>
+      <c r="D12" s="8" t="n">
+        <v>0.916666666666667</v>
+      </c>
+      <c r="E12" s="8" t="n">
+        <v>0.979166666666667</v>
+      </c>
       <c r="F12" s="5" t="n">
         <f aca="false">E12-D12</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="6"/>
-      <c r="B13" s="6"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
+        <v>0.0625</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="7" t="n">
+        <v>43565</v>
+      </c>
+      <c r="D13" s="8" t="n">
+        <v>0.895833333333333</v>
+      </c>
+      <c r="E13" s="8" t="n">
+        <v>0.9375</v>
+      </c>
       <c r="F13" s="5" t="n">
         <f aca="false">E13-D13</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="6"/>
-      <c r="B14" s="6"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
+        <v>0.0416666666666666</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" s="7" t="n">
+        <v>43566</v>
+      </c>
+      <c r="D14" s="8" t="n">
+        <v>0.791666666666667</v>
+      </c>
+      <c r="E14" s="8" t="n">
+        <v>0.833333333333333</v>
+      </c>
       <c r="F14" s="5" t="n">
         <f aca="false">E14-D14</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.0416666666666667</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="6"/>
       <c r="B15" s="6"/>
       <c r="C15" s="7"/>
@@ -733,7 +812,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="6"/>
       <c r="B16" s="6"/>
       <c r="C16" s="7"/>
@@ -744,7 +823,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="6"/>
       <c r="B17" s="6"/>
       <c r="C17" s="7"/>
@@ -755,7 +834,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="6"/>
       <c r="B18" s="6"/>
       <c r="C18" s="7"/>
@@ -766,7 +845,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="6"/>
       <c r="B19" s="6"/>
       <c r="C19" s="7"/>
@@ -777,7 +856,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="6"/>
       <c r="B20" s="6"/>
       <c r="C20" s="7"/>
@@ -788,7 +867,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="6"/>
       <c r="B21" s="6"/>
       <c r="C21" s="7"/>
@@ -799,7 +878,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="6"/>
       <c r="B22" s="6"/>
       <c r="C22" s="7"/>
@@ -810,7 +889,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="6"/>
       <c r="B23" s="6"/>
       <c r="C23" s="7"/>
@@ -821,7 +900,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="6"/>
       <c r="B24" s="6"/>
       <c r="C24" s="7"/>
@@ -832,7 +911,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="6"/>
       <c r="B25" s="6"/>
       <c r="C25" s="7"/>
@@ -843,7 +922,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="6"/>
       <c r="B26" s="6"/>
       <c r="C26" s="7"/>
@@ -854,7 +933,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="6"/>
       <c r="B27" s="6"/>
       <c r="C27" s="7"/>

</xml_diff>